<commit_message>
fix mot so thu
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -374,30 +374,45 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>tgdd_phone</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>tgdd_price</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>tgdd_promotion</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fpt_phone</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>fpt_price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>fpt_promotion</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>vt_phone</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>vt_price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>vt_promotion</t>
         </is>
@@ -414,24 +429,66 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Vivo V17 Pro</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>9.990.000₫</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (500.000₫) cho khách mua online có sinh nhật trong tháng 10
-                    Xem chi tiết
-*
-</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+                            Xem chi tiết
+*
+                        Tặng thêm 1 năm bảo hành chính hãng
+</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Vivo V17 Pro 8GB-128GB</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+9.990.000 ₫
+                Trả góp 0%
+</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%
+Bảo hành 2 năm
+Giảm 30% Sim Viettel khi mua kèm máy
+Tặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Vivo V17 Pro</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>9.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá bán lẻ
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPay
+  Tặng đồng hồ thời trang 3.690.000đ (Áp dụng đến khi hết quà tặng)
+</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -444,20 +501,30 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6.490.000₫</t>
+          <t>Vivo S1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>6.690.000₫</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (350.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 500.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 18 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+                        Giảm ngay 300.000đ (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Vivo S1 6GB-128GB</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t xml:space="preserve">
 6.990.000 ₫
@@ -465,18 +532,36 @@
 </t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 6,490,000đ
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
 Trả góp 0%
+Tặng PMH 300,000đ
 Giảm 30% Sim Viettel khi mua kèm máy
 Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
 </t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Vivo S1</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>6.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Khách hàng lựa chọn 1 trong 2 CTKM sau:
+KM 1: Khách trả thẳng, tặng PMH 300.000đ
+KM 2: Khách trả góp trên giá bán lẻ,Tặng PMH 300.000đ trừ vào tiền trả trước  qua FE hoặc PMHPK 300.000đ qua Home
+  Giảm thêm 5% tối đa 200,000Đ khi thanh toán qua VNPAy
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -489,36 +574,59 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Vivo V15 128GB</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>5.490.000₫</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (330.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-6.490.000 ₫
-                Trả góp 0%
+                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 5,490,000đTrả góp 0%Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+          <t>Vivo V15 6GB-128GB</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 5,490,000đTrả góp 0%Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Vivo V15 128GB</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>6.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Khách hàng lựa chọn 1 trong 2 CTKM sau:
+KM 1: Khách trả thẳng, tặng PMH 1.000.000đ
+KM 2: Khách trả góp trên giá bán lẻ,Tặng PMH 1.000.000đ trừ vào tiền trả trước  hoặc PMHPK 1.000.000đ
+  Giảm giá 5% tối đa 200,000Đ khi thanh toán qua VNPAy
+</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -531,10 +639,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Vivo V15 64GB</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>5.490.000₫</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (280.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -543,7 +656,12 @@
 </t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Vivo V15 6GB-64GB</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 4.990.000 ₫
@@ -553,15 +671,20 @@
 </t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%Giảm ngay 2,000,000đ (Đã trừ vào giá)Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
 </t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -574,30 +697,39 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4.240.000₫</t>
+          <t>Vivo Y17</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>4.990.000₫</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t xml:space="preserve">
 Giảm thêm 5% (250.000₫) cho khách mua online có sinh nhật trong tháng 10
-                            Xem chi tiết
-*
-                        Giảm ngay 300.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 18 - 20/10) (đã trừ vào giá)
-                        Giảm ngay 450.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2.990.000 ₫
-</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+                    Xem chi tiết
+*
+</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Vivo U3</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -610,39 +742,60 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4.390.000₫</t>
+          <t>Vivo Y15</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>4.190.000₫</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (240.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 400.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 18 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-4.790.000 ₫
-                Trả góp 0%
+                        Giảm ngay 200.000đ (đã trừ vào giá)
+                        Giảm ngay 400.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giá đặc biệt khi mua Online đến 20/10: 4,070,000đ
-Trả góp 0%
-Giảm 30% Sim Viettel khi mua kèm máy
-Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+          <t>Vivo Y15 4-64GB</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 4,190,000đTrả góp 0%Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Vivo Y15</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>4.790.000 ₫</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Khách hàng lựa chọn 1 trong 2 CTKM sau:
+KM 1: Khách trả thẳng, tặng PMH 600.000đ
+KM 2: Khách trả góp trên giá bán lẻ,Tặng PMH 600.000đ trừ vào tiền trả trước qua FE  hoặc PMHPK 600.000đ qua Home
+  Giảm thêm 5% tối đa 200,000Đ khi thanh toán qua VNPAy
+</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -655,10 +808,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Vivo Y12</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>3.990.000₫</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (210.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -668,23 +826,51 @@
 </t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Vivo Y12 3GB-64GB</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t xml:space="preserve">
 3.990.000 ₫
+4.190.000₫
+Giảm -5%
                 Trả góp 0%
 </t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Trả góp 0%Giảm ngay 200,000đ (Đã trừ vào giá)Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%
+Giảm ngay 200,000đ (Đã trừ vào giá)
+Giảm 30% Sim Viettel khi mua kèm máy
+Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Vivo Y12</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>4.190.000 ₫</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Khách hàng lựa chọn 1 trong 2 CTKM sau:
+KM 1: Khách trả thẳng, tặng PMH 200.000đ
+KM 2: Khách trả góp trên giá bán lẻ,Tặng PMH 200.000đ trừ vào tiền trả trước  qua FE hoặc PMHPK 200.000đ qua Home
+  Giảm thêm 5% tối đa 200,000Đ khi thanh toán qua VNPAy
+</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -697,43 +883,61 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Vivo Y93</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>2.990.000₫</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (190.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 800.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
+                        Giảm ngay 300.000đ (đã trừ vào giá)
+                        Giảm ngay 500.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
                         *
 </t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-3.790.000 ₫
-                Trả góp 0%
-</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 2,990,000đ
-Hoặc mua giá thường: 3,790,000đ
-Trả góp 0%
-Tặng PMH 300,000đ
-Ưu đãi thêm:
-Giảm 30% Sim Viettel khi mua kèm máy
-Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>Vivo Y93 3-32GB</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 2,990,000đHoặc mua giá thường: 3,790,000đTrả góp 0%Tặng PMH 300,000đƯu đãi thêm:Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Vivo Y93</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>3.790.000 ₫</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Khách hàng lựa chọn 1 trong 2 CTKM sau:
+KM 1: Khách trả thẳng, tặng PMH 800.000đ
+KM 2: Khách trả góp trên giá bán lẻ,Tặng PMH 800.000đ trừ vào tiền trả trước  hoặc PMHPK 800.000đ
+  Giảm thêm 5% tối đa 200,000Đ khi thanh toán qua VNPAy
+</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -746,10 +950,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Vivo Y91C</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>2.590.000₫</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (130.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -758,14 +967,19 @@
 </t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Vivo Y91C 2GB-32GB</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t xml:space="preserve">
 2.590.000 ₫
 </t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm 30% Sim Viettel khi mua kèm máy
@@ -773,8 +987,23 @@
 </t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Vivo Y91C</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2.590.000 ₫</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Giảm thêm 5% tối đa 200,000Đ khi thanh toán qua VNPAy
+</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -787,26 +1016,58 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>OPPO Reno 10x Zoom Edition</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>16.990.000₫</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (1.050.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 4 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
+                        Giảm ngay 3 triệu (đã trừ vào giá)
                         Tặng thêm 1 năm bảo hành hãng
-</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>OPPO Reno Ace</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
       <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Oppo Reno 10x Zoom Edition</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>16.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá giảm )
+  Tặng Phiếu mua hàng 4.000.000đ
+(áp dụng cho đơn hàng đặt và nhận hàng trong ngày 26-31/10) (đã trừ vào giá)
+  Tặng Loa Bluetooth Havit (M76 Hoặc SK579BT)
+  Giảm thêm 10% tối đa không quá 500.000đ khi thanh toán qua VNPAY
+  Bảo hành 2 năm chính Hãng
+  Ưu đãi giảm 40% khi mua Sạc dự phòng (theo phụ lục QĐG phụ kiện)
+</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -817,16 +1078,72 @@
           <t>OPPO Reno2</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>OPPO Reno2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>14.990.000₫</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giảm thêm 5% (750.000₫) cho khách mua online có sinh nhật trong tháng 10
+                    Xem chi tiết
+*
+</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>OPPO Reno2</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+14.990.000 ₫
+                Trả góp 0%
+</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Khách hàng chọn 1 trong 2 khuyến mại sau:
+KM1:
+Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)
+KM2:
+Tặng PMH Phụ Kiện 600,000đ (S)
+Ưu đãi thêm:
+Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>OPPO Reno2</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>14.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá bán lẻ)
+  Tặng Phiếu mua hàng 300.000đ
+  Tặng tai nghe chống ồn Oppo
+  Tặng ốp lưng cao cấp (nằm trong hộp máy)
+  Giảm thêm 10% tối đa không quá 500.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -839,26 +1156,62 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16.990.000₫</t>
+          <t>OPPO Reno</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giảm thêm 5% (1.050.000₫) cho khách mua online có sinh nhật trong tháng 10
+          <t>10.990.000₫</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giảm thêm 5% (650.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 4 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
+                        Giảm ngay 2 triệu (đã trừ vào giá)
                         Tặng thêm 1 năm bảo hành hãng
 </t>
         </is>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Oppo Reno</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 9,990,000đKhách hàng chọn thêm 1 trong 2 khuyến mại sau:KM1 :Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 600,000đ (S) Xem chi tiếtƯu đãi thêm:Bảo hành 2 nămTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Oppo Reno</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>10.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá giảm)
+  Tặng Sạc dự phòng thông minh 10.000mAh (Tekin model Q1031)
+  Tặng Phiếu mua hàng 2.000.000đ (Đã trừ vào giá)
+  Giảm thêm 10% tối đa không quá 500.000đ khi thanh toán qua VNPAY
+  Bảo hành 2 năm chính Hãng
+  Ưu đãi giảm 40% khi mua Sạc dự phòng (theo phụ lục QĐG phụ kiện)
+</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -869,26 +1222,41 @@
           <t xml:space="preserve">OPPO R17 Pro </t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>OPPO R17 Pro</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>OPPO R17 Pro</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 9.990.000 ₫
 </t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm 50% Sim Viettel khi mua kèm máy
 </t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -899,16 +1267,70 @@
           <t>OPPO Reno2 F</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>OPPO Reno2 F</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>8.990.000₫</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giảm thêm 5% (450.000₫) cho khách mua online có sinh nhật trong tháng 10
+                    Xem chi tiết
+*
+</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>OPPO Reno2 F</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+8.990.000 ₫
+                Trả góp 0%
+</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Khách hàng chọn 1 trong 2 khuyến mại sau:
+KM1:
+Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)
+KM2:
+Tặng PMH Phụ Kiện 350,000đ (S)
+Ưu đãi thêm:
+Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>OPPO Reno2 F</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>8.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá bán lẻ)
+  Tặng Phiếu mua hàng 300.000đ
+  Giảm thêm 10% tối đa không quá 500.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -921,39 +1343,62 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>OPPO F11 Pro 128GB</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>7.490.000₫</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (430.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 18 - 20/10) (đã trừ vào giá)
+                        Giảm ngay 500.000đ (đã trừ vào giá)
                         Tặng thêm 1 năm bảo hành hãng
-</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-7.990.000 ₫
-8.490.000₫
-Giảm -6%
-                Trả góp 0%
+                        Giảm ngay 500.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 7,190,000đKhách hàng chọn thêm 1 trong 2 khuyến mại sau:KM1:Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtƯu đãi thêm:Bảo hành 2 nămGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+          <t>OPPO F11 Pro 128GB</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 7,190,000đKhách hàng chọn thêm 1 trong 2 khuyến mại :KM1:Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtƯu đãi thêm:Bảo hành 2 nămGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Oppo F11 Pro 128GB</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>7.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá giảm)
+  Tặng Phiếu mua hàng 1.000.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 26-31/10) (Đã trừ vào giá)
+  Giảm thêm 10% tối đa không quá 500.000đ khi thanh toán qua VNPAY
+  Bảo hành 2 năm chính Hãng
+  Ưu đãi giảm 40% khi mua Sạc dự phòng (theo phụ lục QĐG phụ kiện)
+</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -964,16 +1409,31 @@
           <t>OPPO F11 Pro 64GB</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>OPPO F11 Pro 64GB</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>OPPO K5</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
       <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -986,39 +1446,59 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7.490.000₫</t>
+          <t>OPPO F11</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giảm thêm 5% (430.000₫) cho khách mua online có sinh nhật trong tháng 10
+          <t>6.290.000₫</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giảm thêm 5% (370.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 18 - 20/10) (đã trừ vào giá)
-                        Tặng thêm 1 năm bảo hành hãng
-</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-7.990.000 ₫
-8.490.000₫
-Giảm -6%
-                Trả góp 0%
+                        Giảm ngay 1 triệu (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 7,190,000đKhách hàng chọn thêm 1 trong 2 khuyến mại sau:KM1:Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtƯu đãi thêm:Bảo hành 2 nămGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+          <t>OPPO F11</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 5,990,000đKhách hàng chọn thêm 1 trong 2 khuyến mại sau :KM1:Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtƯu đãi thêm:Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Oppo F11 Pro</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>8.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá bán lẻ
+  Tặng Phiếu mua hàng 1.000.000đ
+  Giảm thêm 10% tối đa không quá 500.000đ khi thanh toán qua VNPAY
+  Ưu đãi giảm 40% khi mua Sạc dự phòng (theo phụ lục QĐG phụ kiện)
+</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1031,10 +1511,15 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>OPPO A9 (2020)</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>6.990.000₫</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (350.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1043,7 +1528,12 @@
 </t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Oppo A9 2020</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t xml:space="preserve">
 6.990.000 ₫
@@ -1051,7 +1541,7 @@
 </t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Khách hàng chọn 1 trong 2 khuyến mại sau :
@@ -1065,8 +1555,13 @@
 </t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1079,10 +1574,15 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>OPPO A5 (2020) 128GB</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>5.290.000₫</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (270.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1091,7 +1591,12 @@
 </t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Oppo A5 2020 4GB-128GB</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t xml:space="preserve">
 5.290.000 ₫
@@ -1099,7 +1604,7 @@
 </t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Khách hàng chọn 1 trong 2 Khuyến mãi sau:
@@ -1112,8 +1617,13 @@
 </t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1126,10 +1636,15 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>OPPO A5 (2020) 64GB</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>4.290.000₫</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (220.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1138,7 +1653,12 @@
 </t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Oppo A5 2020 3GB-64GB</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t xml:space="preserve">
 4.290.000 ₫
@@ -1146,15 +1666,26 @@
 </t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Khách hàng chọn 1 trong 2 khuyến mại sau:KM1:Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:PMH Phụ Kiện 250,000đ (S)Ưu đãi thêm:Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Khách hàng chọn 1 trong 2 khuyến mại sau:
+KM1:
+Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)
+KM2:
+PMH Phụ Kiện 250,000đ (S)
+Ưu đãi thêm:
+Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1167,25 +1698,41 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>OPPO K3</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>5.590.000₫</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (350.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 1,4 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
+                        Giảm ngay 500.000đ (đã trừ vào giá)
+                        Giảm ngay 900.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>OPPO K5</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
       <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1198,10 +1745,15 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>OPPO A5s</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>3.690.000₫</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (190.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1210,7 +1762,12 @@
 </t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>OPPO A5s</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t xml:space="preserve">
 3.690.000 ₫
@@ -1218,7 +1775,7 @@
 </t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Khách hàng chọn 1 trong 2 khuyến mại sau :
@@ -1232,8 +1789,26 @@
 </t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Oppo A5s</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>3.690.000 ₫</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá bán lẻ)
+  Tặng PMH 200.000đ  Hoặc Tặng Sim Viettel F90 (kèm chu kỳ cước tháng đầu tiên)
+  Giảm thêm 5% tối đa không quá 200.000đ khi thanh toán qua VNPAY
+  Ưu đãi giảm 40% khi mua Sạc dự phòng (theo phụ lục QĐG phụ kiện)
+</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1246,10 +1821,15 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>OPPO A1K</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>3.190.000₫</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (160.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1258,7 +1838,12 @@
 </t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>OPPO A1k</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t xml:space="preserve">
 3.190.000 ₫
@@ -1266,15 +1851,33 @@
 </t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Khách hàng chọn 1 trong 2 khuyến mại sau :KM1:Trả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 150,000đ (S) Xem chi tiếtƯu đãi thêm:Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
 </t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Oppo A1K</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>3.190.000 ₫</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá bán lẻ )
+  Tặng Phiếu mua hàng 200.000đ
+  Giảm thêm 5% tối đa không quá 200.000đ khi thanh toán qua VNPAY
+  Ưu đãi giảm 40% khi mua Sạc dự phòng (theo phụ lục QĐG phụ kiện)
+</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1287,26 +1890,47 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>Samsung Galaxy A70</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>8.790.000₫</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (280.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
                         Giảm ngay 500.000đ (đã trừ vào giá)
-                        Phiếu mua hàng Samsung trị giá 150.000đ
-</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+                        Phiếu mua hàng trị giá 150.000đ
+</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A70</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt khi mua Online đến 31/10: 7,490,000đTặng PMH Phụ Kiện 450,000đ (S) Xem chi tiếtHoặc mua giá thường: 8,790,000đTrả góp 0% tặng thêm PMH Phụ Kiện 100,000đ (S) Xem chi tiếtƯu đãi thêm:Tặng PMH Phụ Kiện 200,000đ khi mua OnlineGiảm 30% Sim Viettel khi mua kèm máy
+</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1319,34 +1943,58 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7.990.000₫</t>
+          <t>Samsung Galaxy A50 128GB</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>6.290.000₫</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t xml:space="preserve">
 Giảm thêm 3% (240.000₫) cho khách mua online có sinh nhật trong tháng 10
-                    Xem chi tiết
-*
-</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-7.990.000 ₫
+                            Xem chi tiết
+*
+                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 27 - 31/10) (đã trừ vào giá)
+                        Giảm ngay 700.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 26/10 - 4/11) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Trả góp 0%, mỗi tháng chỉ từ 860,000đGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
-</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
+          <t>Samsung Galaxy A50 (128GB)</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt khi mua Online đến 31/10: 6,290,000đTrả góp 0%, mỗi tháng chỉ từ 860,000đGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
+</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A50 128GB</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>6.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá giảm
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1359,10 +2007,15 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>Samsung Galaxy A50 64GB</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>6.990.000₫</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (210.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1371,16 +2024,33 @@
 </t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-9.990.000 ₫
-</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A51</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
       <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A50 64GB</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>6.090.000 ₫</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá giảm
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1393,39 +2063,60 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>7.790.000₫</t>
+          <t>Samsung Galaxy A50s</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
+        <is>
+          <t>5.890.000₫</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (240.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Mua kèm Vòng đeo tay thông minh Galaxy Fit E màu đen ưu đãi chỉ 99,000đ
-                        Giảm ngay 500.000đ qua quà tặng Galaxy   Xem chi tiết
+                        Giảm ngay 800.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 27/10 - 31/10) (đã trừ vào giá)
                         Ưu đãi quà tặng độc quyền Galaxy trị giá đến 450.000đ   Xem chi tiết
+                        Giảm ngay 1,1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 30 - 31/10) (đã trừ vào giá)
                         Phiếu mua hàng Samsung trị giá 100.000đ
 </t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-7.790.000 ₫
-                Trả góp 0%
-</t>
-        </is>
-      </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Khuyến mại:Giảm ngay 500,000đ (Quà tặng Galaxy)Tăng Gear Fit E BlackƯu đãi quà tặng độc quyền Galaxy trị giá đến 450.000đ Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyKhách hàng chọn 1 trong 2 khuyến mại sau:KM1:Trả góp 0%, trả trước chỉ từ 779,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
+          <t>Samsung Galaxy A50s</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 6,490,000đTặng sạc dự phòng chính hãng Samsung 10.000mAhƯu đãi quà tặng độc quyền Galaxy trị giá đến 450.000đ Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyKhách hàng chọn thêm 1 trong 2 khuyến mại sau:KM1:Trả góp 0%, trả trước chỉ từ 779,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A50s</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>6.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá giảm
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1438,10 +2129,15 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>Samsung Galaxy A50 64GB</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>6.990.000₫</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (210.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1450,16 +2146,33 @@
 </t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-9.990.000 ₫
-</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A51</t>
+        </is>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
       <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A50 64GB</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>6.090.000 ₫</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá giảm
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1472,10 +2185,15 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>6.290.000₫</t>
+          <t>Samsung Galaxy A30s</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
+        <is>
+          <t>5.390.000₫</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (190.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1483,26 +2201,32 @@
 *
                         Giảm ngay 300.000đ qua quà tặng Galaxy   Xem chi tiết
                         Ưu đãi quà tặng Galaxy trị giá đến 360.000đ   Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-6.290.000 ₫
-                Trả góp 0%
+                        Giảm ngay 900.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 30 - 31/10) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Khách hàng chọn 1 trong 2 khuyến mại sau :KM1:Trả góp 0%, mỗi tháng chỉ từ 774,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtƯu đãi thêm:Giảm ngay 300,000đ (Quà tặng Galaxy)Ưu đãi quà tặng độc quyền Galaxy trị giá đến 360.000đ Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
-</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
+          <t>Samsung Galaxy A30s</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt khi mua Online đến 31/10: 5,790,000đTặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtHoặc mua giá thường: 6,290,000đTrả góp 0%, mỗi tháng chỉ từ 774,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)Ưu đãi thêm:Giảm ngay 300,000đ (Quà tặng Galaxy)Ưu đãi quà tặng độc quyền Galaxy trị giá đến 360.000đ Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
+</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1515,35 +2239,56 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4.990.000₫</t>
+          <t>Samsung Galaxy A30</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giảm thêm 3% (150.000₫) cho khách mua online có sinh nhật trong tháng 10
-                    Xem chi tiết
-*
-</t>
+          <t>5.290.000₫</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
           <t xml:space="preserve">
-6.290.000 ₫
-                Trả góp 0%
+Giảm thêm 3% (180.000₫) cho khách mua online có sinh nhật trong tháng 10
+                            Xem chi tiết
+*
+                        Giảm ngay 500.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 26/10 - 4/11) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Khách hàng chọn 1 trong 2 khuyến mại sau :KM1:Trả góp 0%, mỗi tháng chỉ từ 774,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtƯu đãi thêm:Giảm ngay 300,000đ (Quà tặng Galaxy)Ưu đãi quà tặng độc quyền Galaxy trị giá đến 360.000đ Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
-</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
+          <t>Samsung Galaxy A30s</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt khi mua Online đến 31/10: 5,790,000đTặng PMH Phụ Kiện 350,000đ (S) Xem chi tiếtHoặc mua giá thường: 6,290,000đTrả góp 0%, mỗi tháng chỉ từ 774,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)Ưu đãi thêm:Giảm ngay 300,000đ (Quà tặng Galaxy)Ưu đãi quà tặng độc quyền Galaxy trị giá đến 360.000đ Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
+</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A30 4GB/64GB</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>4.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Giảm giá 5% tối đa 200.000đ khi thanh toán qua VNPay
+</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1556,28 +2301,51 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>4.990.000₫</t>
+          <t>Samsung Galaxy A30 3GB/32GB</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>4.490.000₫</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t xml:space="preserve">
 Giảm thêm 3% (150.000₫) cho khách mua online có sinh nhật trong tháng 10
-                    Xem chi tiết
-*
-</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-9.990.000 ₫
-</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
+                            Xem chi tiết
+*
+                        Giảm ngay 500.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 26/10 - 4/11) (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A51</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
       <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A30 3GB/32GB</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>4.590.000 ₫</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Tặng Gói cước khổng lồ miễn phí 10 Phút nội mạng (1 tháng chu kỳ Sim F90)
+  Giảm giá 5% tối đa 200.000đ khi thanh toán qua VNPay
+</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1590,19 +2358,30 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>4.490.000₫</t>
+          <t>Samsung Galaxy M20</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>3.990.000₫</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t xml:space="preserve">
 Giảm thêm 3% (140.000₫) cho khách mua online có sinh nhật trong tháng 10
-                    Xem chi tiết
-*
-</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
+                            Xem chi tiết
+*
+                        Giảm ngay 500.000đ (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy M20</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t xml:space="preserve">
 3.990.000 ₫
@@ -1611,15 +2390,20 @@
 </t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Giảm ngay 1,000,000đ (đã trừ vào giá)Tặng Sạc Dự Phòng chính hãng Samsung 10.000mAh (áp dụng đến 20/10)Tặng PMH Phụ Kiện 150,000đ (S) Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
-</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giảm ngay 1,000,000đ (đã trừ vào giá)Tặng PMH Phụ Kiện 150,000đ (S) Xem chi tiếtGiảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
+</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1632,10 +2416,15 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>Samsung Galaxy A20</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t>4.190.000₫</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (130.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1644,12 +2433,33 @@
 </t>
         </is>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A20</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+4.190.000 ₫
+                Trả góp 0%
+</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Khách hàng chọn 1 trong 2 khuyến mại sau :KM1:Trả góp 0%, mỗi tháng chỉ từ 774,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 250,000đ (S) Xem chi tiếtƯu đãi thêm:Giảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 200,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
+</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1662,10 +2472,15 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>Samsung Galaxy A10</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>3.090.000₫</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 3% (100.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1674,12 +2489,42 @@
 </t>
         </is>
       </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A10</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+3.090.000 ₫
+</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Khách hàng chọn 1 trong 2 khuyến mại sau :KM1:Trả góp 0%, mỗi tháng chỉ 380,000đ tặng thêm PMH Phụ Kiện 100,000đ (S)KM2:Tặng PMH Phụ Kiện 150,000đ (S) Xem chi tiếtƯu đãi thêm:Giảm 30% Sim Viettel khi mua kèm máyGiảm thêm đến 150,000đ khi thanh toán 100% giá trị đơn hàng qua VNPay-QR
+</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A10</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>2.890.000 ₫</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Giảm thêm 5% tối đa 200.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1692,10 +2537,15 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>Huawei Y9 Prime (2019)</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
           <t>5.840.000₫</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (330.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1705,14 +2555,20 @@
 </t>
         </is>
       </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1725,10 +2581,15 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>Huawei P30 Pro</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t>20.690.000₫</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (1.150.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1738,7 +2599,12 @@
 </t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Huawei P30 Pro</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t xml:space="preserve">
 20.690.000 ₫
@@ -1747,7 +2613,7 @@
 </t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm ngay 2,300,000đ (đã trừ vào giá)
@@ -1755,8 +2621,13 @@
 </t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1769,10 +2640,15 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>Huawei P30 Lite</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t>6.020.000₫</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (340.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1782,7 +2658,12 @@
 </t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Huawei P30 Lite</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t xml:space="preserve">
 6.020.000 ₫
@@ -1792,7 +2673,7 @@
 </t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%
@@ -1802,8 +2683,25 @@
 </t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Huawei P30 Lite</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>6.690.000 ₫</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá bán lẻ
+  Tặng PMH 670.000đ
+  Giảm thêm 10% tối đa 500.000Đ khi thanh toán qua VNPay
+</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1816,20 +2714,104 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>4.490.000₫</t>
+          <t>Huawei Nova 3i</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
+        <is>
+          <t>5.390.000₫</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (300.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
+                        Giảm ngay 600.000đ (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Huawei Nova 3i</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+5.390.000 ₫
+5.990.000₫
+Giảm -10%
+                Trả góp 0%
+</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%
+Giảm ngay 600,000đ (đã trừ vào giá)
+Giảm 30% Sim Viettel khi mua kèm máy
+Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Huawei Nova 3i</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>5.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá bán lẻ
+  Tặng PMH 600.000đ
+  Giảm thêm 10 % tối đa 500.000Đ khi thanh toán qua VNPay
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Huawei Nova 3i Trắng</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Huawei Nova 3i Trắng</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>4.490.000₫</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giảm thêm 5% (300.000₫) cho khách mua online có sinh nhật trong tháng 10
+                            Xem chi tiết
+*
                         Giảm ngay 1,5 triệu (đã trừ vào giá)
 </t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Huawei Nova 3i Trắng</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t xml:space="preserve">
 4.490.000 ₫
@@ -1839,7 +2821,7 @@
 </t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%
@@ -1849,55 +2831,13 @@
 </t>
         </is>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Huawei Nova 3i Trắng</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>4.490.000₫</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Giảm thêm 5% (300.000₫) cho khách mua online có sinh nhật trong tháng 10
-                            Xem chi tiết
-*
-                        Giảm ngay 1,5 triệu (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-4.490.000 ₫
-5.990.000₫
-Giảm -25%
-                Trả góp 0%
-</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Trả góp 0%
-Giảm ngay 1,500,000đ (đã trừ vào giá)
-Giảm 30% Sim Viettel khi mua kèm máy
-Tặng mã giảm giá 5% để mua Laptop
-</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1910,10 +2850,15 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>Huawei Y9 Prime (2019)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>5.840.000₫</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (330.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1923,7 +2868,12 @@
 </t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Huawei Y9 Prime (2019)</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t xml:space="preserve">
 5.840.000 ₫
@@ -1933,7 +2883,7 @@
 </t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%
@@ -1943,8 +2893,25 @@
 </t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Huawei Y9 Prime (2019)</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>6.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% trên giá bán lẻ
+  Tặng PMH 650.000đ
+  Giảm thêm 10% tối đa 500.000Đ khi thanh toán qua VNPay
+</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1957,10 +2924,15 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>Huawei Y9 (2019)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
           <t>4.990.000₫</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (250.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -1969,28 +2941,28 @@
 </t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-5.840.000 ₫
-6.490.000₫
-Giảm -10%
-                Trả góp 0%
-</t>
-        </is>
-      </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Trả góp 0%
-Giảm ngay 650,000đ (đã trừ vào giá)
-Giảm 30% Sim Viettel khi mua kèm máy
-Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
+          <t>Huawei Y9 (2019)</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 4,490,000đGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2003,10 +2975,15 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>Xiaomi Mi 9T</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>7.990.000₫</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (400.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2015,7 +2992,12 @@
 </t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi 9T 128GB</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t xml:space="preserve">
 8.490.000 ₫
@@ -2025,15 +3007,31 @@
 </t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Trả góp 0%Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%
+Bảo hành 18 tháng
+Giảm 30% Sim Viettel khi mua kèm máy
+Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>7.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp lãi suất 0% 
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPay
+  Bảo hành 18 tháng
+</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2046,21 +3044,31 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>Xiaomi Mi 9 SE</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>6.490.000₫</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (430.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
                         Giảm ngay 1 triệu (đã trừ vào giá)
-                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 17 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
+                        Giảm ngay 1 triệu (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
+</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi 9 SE 64GB</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
         <is>
           <t xml:space="preserve">
 7.490.000 ₫
@@ -2068,15 +3076,30 @@
 </t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%Tặng PMH 1,000,000đBảo hành 18 thángTặng mã giảm giá 5% để mua Laptop Xem chi tiết
 </t>
         </is>
       </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi 9 SE 6/64GB</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>7.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Giảm thêm 10% tối đa 500.000đ khi thanh toán qua VNPay
+</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2087,20 +3110,35 @@
           <t xml:space="preserve">Xiaomi Mi 8 Lite </t>
         </is>
       </c>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi 8 Lite</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi 8 Lite 64GB</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t xml:space="preserve">
 3.990.000 ₫
 </t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2113,10 +3151,15 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi Note 8 Pro (6GB/64GB)</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>5.990.000₫</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (300.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2125,7 +3168,12 @@
 </t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 8 Pro 6GB-128GB</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t xml:space="preserve">
 6.990.000 ₫
@@ -2133,7 +3181,7 @@
 </t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%
@@ -2142,8 +3190,13 @@
 </t>
         </is>
       </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2156,10 +3209,15 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi Note 8 (4GB/128GB)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
           <t>5.490.000₫</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (280.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2168,25 +3226,33 @@
 </t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-6.990.000 ₫
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 8 4GB-128GB</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+5.490.000 ₫
                 Trả góp 0%
 </t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Trả góp 0%
-Bảo hành 18 tháng
-Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%Bảo hành 18 thángTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2199,10 +3265,15 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi Note 8 (4GB/64GB)</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
           <t>4.990.000₫</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (250.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2211,12 +3282,22 @@
 </t>
         </is>
       </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi Note 8 4GB-64GB</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
       <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2229,36 +3310,47 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi Note 7 (4GB/64GB)</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
           <t>4.490.000₫</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (250.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
-                        Giảm ngay 500.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 19 - 20/10) (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-4.690.000 ₫
-                Trả góp 0%
+                        Giảm ngay 300.000đ (đã trừ vào giá)
+                        Giảm ngay 200.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
 </t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 4,490,000đTrả góp 0%Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
+          <t>Xiaomi Redmi Note 7 64GB</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 4,490,000đTrả góp 0%Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2271,10 +3363,15 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi 7 (3GB/32GB)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
           <t>3.290.000₫</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (190.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2284,22 +3381,33 @@
 </t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2.190.000 ₫
-</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+          <t>Xiaomi Redmi 7 3GB-32GB</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+3.290.000 ₫
+                Trả góp 0%
+</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2312,10 +3420,15 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi 7 (2GB/16GB)</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>2.690.000₫</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (150.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2325,22 +3438,32 @@
 </t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi 7 2GB-16GB</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t xml:space="preserve">
 2.690.000 ₫
 </t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Giá đặc biệt đến 20/10: 2,490,000đBảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2353,10 +3476,15 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>Xiaomi Redmi 7A (2GB/32GB)</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>2.190.000₫</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (110.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2365,22 +3493,32 @@
 </t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Xiaomi Redmi 7A 32GB</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t xml:space="preserve">
 2.190.000 ₫
 </t>
         </is>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Bảo hành 18 thángGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
 </t>
         </is>
       </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2393,10 +3531,15 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>Realme 5 Pro (8GB/128GB)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>6.990.000₫</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (350.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2405,7 +3548,12 @@
 </t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Realme 5 Pro 8GB-128GB</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t xml:space="preserve">
 6.990.000 ₫
@@ -2413,15 +3561,32 @@
 </t>
         </is>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
 </t>
         </is>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Realme 5 Pro 8GB-128GB</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>6.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% (làm HĐ trên giá bán lẻ)
+  Tặng Phiếu mua hàng 200.000đ
+  Giảm thêm 5% tối đa không quá 200.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2434,10 +3599,15 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>Realme 5 (4GB/128GB)</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
           <t>4.990.000₫</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (250.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2447,7 +3617,12 @@
 </t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Realme 5 Pro 4GB-128GB</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t xml:space="preserve">
 5.990.000 ₫
@@ -2455,7 +3630,7 @@
 </t>
         </is>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="H54" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%
@@ -2464,8 +3639,13 @@
 </t>
         </is>
       </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2478,10 +3658,15 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>Realme 5 (3GB/64GB)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
           <t>3.990.000₫</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (200.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2490,7 +3675,12 @@
 </t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Realme 5 3GB-64GB</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t xml:space="preserve">
 3.990.000 ₫
@@ -2498,7 +3688,7 @@
 </t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Trả góp 0%
@@ -2507,8 +3697,24 @@
 </t>
         </is>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Realme 5 3GB-64GB</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>3.990.000 ₫</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% 
+  Giảm thêm 5% tối đa không quá 200.000đ khi thanh toán qua VNPAY
+</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2521,10 +3727,15 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>Realme 3 Pro (4GB/64GB)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
           <t>4.990.000₫</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (300.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2534,25 +3745,40 @@
 </t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-5.490.000 ₫
-6.490.000₫
-Giảm -15%
-                Trả góp 0%
-</t>
-        </is>
-      </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Trả góp 0%Giảm ngay 1,000,000đ (Đã trừ vào giá)Bảo hành 2 nămGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
+          <t>Realme 3 Pro 4GB-64GB</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 4,990,000đTrả góp 0%Bảo hành 2 nămGiảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Realme 3 Pro 128GB</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>7.490.000 ₫</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+  Trả góp 0% hoặc Tặng Phiếu mua hàng 1.500.000đ (Chỉ áp dụng cho khách hàng mua online)
+  Giảm thêm 10% không quá 200.000đ khi thanh toán qua VNPAY
+  1 đổi 1 trong 30 ngày đối với những máy lỗi do nhà sản xuất
+</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2565,38 +3791,53 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>4.490.000₫</t>
+          <t>Realme 3 (4GB/64GB)</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
+        <is>
+          <t>4.290.000₫</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (250.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
                         Giảm ngay 500.000đ (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-3.990.000 ₫
+                        Giảm ngay 200.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
+                        *
+</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Realme 3 4GB-64GB</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+4.490.000 ₫
                 Trả góp 0%
 </t>
         </is>
       </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-Trả góp 0%
-Giảm 30% Sim Viettel khi mua kèm máy
-Tặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="inlineStr"/>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Trả góp 0%Giảm ngay 500,000đ (Đã trừ vào giá)Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
+</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2609,37 +3850,48 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>3.490.000₫</t>
+          <t>Realme 3 (3GB/32GB)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
+        <is>
+          <t>3.190.000₫</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (200.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
                         Giảm ngay 500.000đ (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-2.590.000 ₫
-2.990.000₫
-Giảm -13%
+                        Giảm ngay 300.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
+                        *
 </t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop Xem chi tiết
-</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="inlineStr"/>
+          <t>Realme 3 3GB-32GB</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Giá đặc biệt đến 31/10: 3,190,000đHoặc mua giá thường: 3,490,000đTrả góp 0%Ưu đãi thêm:Giảm 30% Sim Viettel khi mua kèm máyTặng mã giảm giá 5% để mua Laptop
+</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2652,27 +3904,40 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2.990.000₫</t>
+          <t>Realme C2 (3GB/32GB)</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
+        <is>
+          <t>2.790.000₫</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (170.000₫) cho khách mua online có sinh nhật trong tháng 10
                             Xem chi tiết
 *
                         Giảm ngay 300.000đ (đã trừ vào giá)
-</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="inlineStr"/>
+                        Giảm ngay 200.000đ (áp dụng cho đơn hàng đặt và nhận hàng trong ngày 28 - 31/10) (đã trừ vào giá)
+                        *
+</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2685,10 +3950,15 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t>Realme C2 (2GB/16GB)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>2.290.000₫</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t xml:space="preserve">
 Giảm thêm 5% (130.000₫) cho khách mua online có sinh nhật trong tháng 10
@@ -2698,14 +3968,20 @@
 </t>
         </is>
       </c>
-      <c r="E60" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>